<commit_message>
added all the names
</commit_message>
<xml_diff>
--- a/Manipulating Excels with Code/shared_excel.xlsx
+++ b/Manipulating Excels with Code/shared_excel.xlsx
@@ -9,7 +9,7 @@
     <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -427,7 +427,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -472,7 +472,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>CHLOE LA FOLLE</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
ajout de la liste des joueurs
</commit_message>
<xml_diff>
--- a/Manipulating Excels with Code/shared_excel.xlsx
+++ b/Manipulating Excels with Code/shared_excel.xlsx
@@ -1,33 +1,77 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comet\Desktop\Bureau\Code Work\manipulating_excels\Manipulating Excels with Code\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D7D445-C479-4368-AFD5-11286C935878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="30015" yWindow="4170" windowWidth="19830" windowHeight="14970" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="30015" yWindow="4170" windowWidth="19830" windowHeight="14970" xr2:uid="{954FDF21-168F-45AB-B23A-57329EC4B510}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>Nom de la BDF</t>
+  </si>
+  <si>
+    <t>Classement</t>
+  </si>
+  <si>
+    <t>Joueur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heure </t>
+  </si>
+  <si>
+    <t>Killer</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,80 +90,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -419,72 +404,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1509B223-D6B0-43C2-AA9F-A598451C8D97}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="21.42578125" customWidth="1" min="1" max="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Nom de la BDF</t>
-        </is>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Classement</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Joueur</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Heure </t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Killer</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Points</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>CHLOE LA FOLLE</t>
-        </is>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
-    <oddHeader/>
-    <oddFooter>&amp;C&amp;"Calibri"&amp;6 &amp;K626469_x000d_# Public</oddFooter>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;K626469 Public</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
its working better still huge bugs
</commit_message>
<xml_diff>
--- a/Manipulating Excels with Code/shared_excel.xlsx
+++ b/Manipulating Excels with Code/shared_excel.xlsx
@@ -1,37 +1,72 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comet\Desktop\Bureau\Code Work\manipulating_excels\Manipulating Excels with Code\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30120E7F-B221-4E1F-BEB1-596650BDF30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="12690" yWindow="5175" windowWidth="21945" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+  <si>
+    <t>Classement</t>
+  </si>
+  <si>
+    <t>Joueur</t>
+  </si>
+  <si>
+    <t>Heure</t>
+  </si>
+  <si>
+    <t>Killer</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>Côme</t>
+  </si>
+  <si>
+    <t>Hugo D</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +81,44 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,44 +406,58 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Classement</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Joueur</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Heure</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Killer</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Points</t>
-        </is>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2">
+        <v>45541.32284073528</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2">
+        <v>45541.32284073528</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected the bug it seems (more test are necessary)
</commit_message>
<xml_diff>
--- a/Manipulating Excels with Code/shared_excel.xlsx
+++ b/Manipulating Excels with Code/shared_excel.xlsx
@@ -16,9 +16,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -58,12 +57,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,112 +438,56 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Nom de la BDF</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 1</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 2</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 3</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 4</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Classement</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Joueur</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Heure</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Killer</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Points</t>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Classement des éliminés</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>Classement</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>Joueur</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Heure </t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>Heure</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
         <is>
           <t>Killer</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="1" t="inlineStr">
         <is>
           <t>Points</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Côme</t>
         </is>
       </c>
-      <c r="H3" s="2" t="n">
-        <v>45542.66999538201</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Mathieu</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr"/>
+      <c r="C3" s="3" t="n">
+        <v>45542.70299954861</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Eric</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
created something for the upload of the users
</commit_message>
<xml_diff>
--- a/Manipulating Excels with Code/shared_excel.xlsx
+++ b/Manipulating Excels with Code/shared_excel.xlsx
@@ -16,9 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -57,13 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,7 +436,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Classement des éliminés</t>
+          <t xml:space="preserve">BDF Edition 9 </t>
         </is>
       </c>
     </row>
@@ -457,7 +453,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>Heure</t>
+          <t xml:space="preserve">Heure </t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
@@ -473,20 +469,42 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Côme</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>45542.70299954861</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Eric</t>
-        </is>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a correction for the date blocking the app
</commit_message>
<xml_diff>
--- a/Manipulating Excels with Code/shared_excel.xlsx
+++ b/Manipulating Excels with Code/shared_excel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,7 +453,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Heure </t>
+          <t>Heure</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
@@ -505,6 +505,46 @@
     <row r="10">
       <c r="A10" t="n">
         <v>8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>8</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Côme</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>09:29</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Côme</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>9</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Baptiste</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>09:30</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Mathieu</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
now its uploaded in the right order
</commit_message>
<xml_diff>
--- a/Manipulating Excels with Code/shared_excel.xlsx
+++ b/Manipulating Excels with Code/shared_excel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,7 +453,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>Heure</t>
+          <t xml:space="preserve">Heure </t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
@@ -496,54 +496,44 @@
       <c r="A8" t="n">
         <v>6</v>
       </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Côme</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Mathieu</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>7</v>
       </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Côme</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Didier</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
         <v>8</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>8</v>
-      </c>
-      <c r="B11" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>Côme</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>09:29</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Côme</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>9</v>
-      </c>
-      <c r="B12" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>Baptiste</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>09:30</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Mathieu</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added the hour still some changes to make
</commit_message>
<xml_diff>
--- a/Manipulating Excels with Code/shared_excel.xlsx
+++ b/Manipulating Excels with Code/shared_excel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,6 +466,11 @@
           <t>Points</t>
         </is>
       </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>Heure</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -476,21 +481,81 @@
       <c r="A4" t="n">
         <v>2</v>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Côme</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Sylvie P</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>13:57</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>3</v>
       </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Côme</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Côme</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>4</v>
       </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Côme</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Hugo D</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>13:55</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>5</v>
       </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Côme</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Eric</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>13:55</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -503,7 +568,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Mathieu</t>
+          <t>Eric</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>13:55</t>
         </is>
       </c>
     </row>
@@ -518,7 +588,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Didier</t>
+          <t>Côme</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>13:55</t>
         </is>
       </c>
     </row>
@@ -533,7 +608,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Baptiste</t>
+          <t>Côme</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>13:55</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added the point system
</commit_message>
<xml_diff>
--- a/Manipulating Excels with Code/shared_excel.xlsx
+++ b/Manipulating Excels with Code/shared_excel.xlsx
@@ -476,36 +476,162 @@
       <c r="A3" t="n">
         <v>1</v>
       </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Côme</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Eric</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>10</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>2</v>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Côme</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Baptiste</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>6</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>3</v>
       </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Côme</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Baptiste</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>4</v>
       </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Côme</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Baptiste</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>5</v>
       </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Côme</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Baptiste</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>6</v>
       </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Côme</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Baptiste</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>7</v>
       </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Côme</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Baptiste</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>11:01</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -513,17 +639,20 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Didier</t>
+          <t>Côme</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Mathieu</t>
-        </is>
+          <t>Baptiste</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>07:52</t>
+          <t>11:01</t>
         </is>
       </c>
     </row>
@@ -533,17 +662,20 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Hugo D</t>
+          <t>Côme</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Didier</t>
-        </is>
+          <t>Baptiste</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>07:48</t>
+          <t>11:01</t>
         </is>
       </c>
     </row>
@@ -553,17 +685,20 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Anne-Lise</t>
+          <t>Côme</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Didier</t>
-        </is>
+          <t>Baptiste</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>07:47</t>
+          <t>11:01</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
corrected a lot of things and now it seems like its properly working
</commit_message>
<xml_diff>
--- a/Manipulating Excels with Code/shared_excel.xlsx
+++ b/Manipulating Excels with Code/shared_excel.xlsx
@@ -476,23 +476,8 @@
       <c r="A3" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Côme</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Eric</t>
-        </is>
-      </c>
       <c r="E3" t="n">
-        <v>10</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>11:01</t>
-        </is>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -501,20 +486,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Côme</t>
+          <t>Didier</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Baptiste</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>6</v>
+          <t>Eric</t>
+        </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>11:01</t>
+          <t>10:05</t>
         </is>
       </c>
     </row>
@@ -524,20 +506,20 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Côme</t>
+          <t>Baptiste</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Baptiste</t>
+          <t>Didier</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>11:01</t>
+          <t>10:05</t>
         </is>
       </c>
     </row>
@@ -552,15 +534,15 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Baptiste</t>
+          <t>Didier</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>11:01</t>
+          <t>10:05</t>
         </is>
       </c>
     </row>
@@ -570,20 +552,20 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Côme</t>
+          <t>Sylvie P</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Baptiste</t>
+          <t>Didier</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>11:01</t>
+          <t>10:04</t>
         </is>
       </c>
     </row>
@@ -593,20 +575,20 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Côme</t>
+          <t>Béa</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Baptiste</t>
+          <t>Didier</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>11:01</t>
+          <t>10:04</t>
         </is>
       </c>
     </row>
@@ -616,12 +598,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Côme</t>
+          <t>Anne-Lise</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Baptiste</t>
+          <t>Didier</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -629,7 +611,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>11:01</t>
+          <t>10:04</t>
         </is>
       </c>
     </row>
@@ -639,12 +621,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Côme</t>
+          <t>Mathieu</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Baptiste</t>
+          <t>Eric</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -652,7 +634,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>11:01</t>
+          <t>10:04</t>
         </is>
       </c>
     </row>
@@ -662,12 +644,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Côme</t>
+          <t>Jean Rob</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Baptiste</t>
+          <t>Eric</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -675,7 +657,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>11:01</t>
+          <t>10:04</t>
         </is>
       </c>
     </row>
@@ -685,12 +667,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Côme</t>
+          <t>Hugo D</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Baptiste</t>
+          <t>Jean Rob</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -698,7 +680,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>11:01</t>
+          <t>10:03</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Well it seems like we have a MVP
</commit_message>
<xml_diff>
--- a/Manipulating Excels with Code/shared_excel.xlsx
+++ b/Manipulating Excels with Code/shared_excel.xlsx
@@ -476,6 +476,11 @@
       <c r="A3" t="n">
         <v>1</v>
       </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Eric</t>
+        </is>
+      </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
@@ -494,9 +499,12 @@
           <t>Eric</t>
         </is>
       </c>
+      <c r="E4" t="n">
+        <v>10</v>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>10:05</t>
+          <t>10:15</t>
         </is>
       </c>
     </row>
@@ -515,11 +523,11 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>10:05</t>
+          <t>10:15</t>
         </is>
       </c>
     </row>
@@ -538,11 +546,11 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>10:05</t>
+          <t>10:15</t>
         </is>
       </c>
     </row>
@@ -561,11 +569,11 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>10:04</t>
+          <t>10:15</t>
         </is>
       </c>
     </row>
@@ -584,11 +592,11 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>10:04</t>
+          <t>10:15</t>
         </is>
       </c>
     </row>
@@ -611,7 +619,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>10:04</t>
+          <t>10:14</t>
         </is>
       </c>
     </row>
@@ -634,7 +642,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>10:04</t>
+          <t>10:14</t>
         </is>
       </c>
     </row>
@@ -657,7 +665,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>10:04</t>
+          <t>10:14</t>
         </is>
       </c>
     </row>
@@ -680,7 +688,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>10:03</t>
+          <t>10:14</t>
         </is>
       </c>
     </row>

</xml_diff>